<commit_message>
Some new spells added
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/hexes.xlsx
+++ b/CoreRulebook/Data/Spells/hexes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="173">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -950,6 +950,27 @@
   </si>
   <si>
     <t xml:space="preserve">If the spell makes contact with matter, causes it to instantly disintegrate. Living beings take 10d10 worth of force damage. Resist for half damage. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Howl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{\bf Werewolf Species spell. This spell can only be learned by werewolves} \\ Release an earsplitting, supernatural roar which causes all beings within 100m to perform a SPR Resist. Failure causes them to gain the {\it Terrified} status. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lombus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue bolt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The target suffers a 1-point penalty to all checks for the duration of the spell. </t>
   </si>
 </sst>
 </file>
@@ -1105,14 +1126,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1126,6 +1147,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="87.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="26.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="12" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,6 +2205,64 @@
       </c>
       <c r="J34" s="4" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>